<commit_message>
IEEE13 balanced feeder updates
Fixed the mismatch of a rotated vector that was cuasing problems in the balanced IEEE13 node feeder
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>Test Settings (read this into RTlab)</t>
   </si>
@@ -145,9 +145,6 @@
     <t>T3.1</t>
   </si>
   <si>
-    <t>12:00-12:06</t>
-  </si>
-  <si>
     <t>33/P1,33/Q1</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>12:00-13:00</t>
   </si>
   <si>
-    <t>T3.1 (old)</t>
-  </si>
-  <si>
     <t>T3.2</t>
   </si>
   <si>
@@ -218,6 +212,114 @@
   </si>
   <si>
     <t>units: kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T3.2_unbalanced </t>
+  </si>
+  <si>
+    <t>T3.2_unbalanced.mat</t>
+  </si>
+  <si>
+    <t>652/P1,652/Q1</t>
+  </si>
+  <si>
+    <t>12:00-12:05</t>
+  </si>
+  <si>
+    <t>T3_1_33.mat</t>
+  </si>
+  <si>
+    <t>PlotLocalControl1</t>
+  </si>
+  <si>
+    <t>kgains</t>
+  </si>
+  <si>
+    <t>T3.1_33abc</t>
+  </si>
+  <si>
+    <t>T3.1_33a</t>
+  </si>
+  <si>
+    <t>33/P1,33/Q1,33/P2,33/Q2,33/P3,33/Q3</t>
+  </si>
+  <si>
+    <t>6_a,6_b,6_c</t>
+  </si>
+  <si>
+    <t>T3.1_33b</t>
+  </si>
+  <si>
+    <t>T3_1_33b.mat</t>
+  </si>
+  <si>
+    <t>33/P2,33/Q2</t>
+  </si>
+  <si>
+    <t>33/P3,33/Q3</t>
+  </si>
+  <si>
+    <t>T3_1_33c.mat</t>
+  </si>
+  <si>
+    <t>T3.1_33c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ku = 5, Tu = 2; Ku = 0 Tu=2 </t>
+  </si>
+  <si>
+    <t>PlotLocalControl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ku = 5, Tu = 1; Ku = 0 Tu=2 </t>
+  </si>
+  <si>
+    <t>T3.1_33ab</t>
+  </si>
+  <si>
+    <t>T3_1_33ab.mat</t>
+  </si>
+  <si>
+    <t>33/P1,33/Q1,33/P2,33/Q2</t>
+  </si>
+  <si>
+    <t>T3.1_33bc</t>
+  </si>
+  <si>
+    <t>T3_1_33bc.mat</t>
+  </si>
+  <si>
+    <t>33/P2,33/Q2,33/P3,33/Q3</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>T3.1_33ac</t>
+  </si>
+  <si>
+    <t>T3_1_33ac.mat</t>
+  </si>
+  <si>
+    <t>33/P1,33/Q1,33/P3,33/Q3</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>test idx</t>
+  </si>
+  <si>
+    <t>ku=0.5,Tu=2;Ku=0.02,Tu=2</t>
+  </si>
+  <si>
+    <t>same as T3.2^</t>
+  </si>
+  <si>
+    <t>T5.1</t>
+  </si>
+  <si>
+    <t>T5_1.mat</t>
   </si>
 </sst>
 </file>
@@ -500,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -619,6 +721,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -906,43 +1011,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="H7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="4" width="16.46484375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.73046875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.53125" style="4" customWidth="1"/>
+    <col min="1" max="4" width="16.36328125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.6328125" style="4" customWidth="1"/>
     <col min="7" max="8" width="51" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16.46484375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="11.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.19921875" style="4"/>
+    <col min="9" max="9" width="43.54296875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.08984375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.65" thickBot="1">
+    <row r="1" spans="1:16" ht="15" thickBot="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:11" ht="28.9" thickBot="1">
+    <row r="2" spans="1:16" ht="29.5" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>2</v>
@@ -960,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>6</v>
@@ -968,13 +1073,19 @@
       <c r="J2" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="85.9" thickBot="1">
+      <c r="K2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="102" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="7" t="s">
@@ -990,16 +1101,19 @@
         <v>18</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.9" thickBot="1">
+        <v>61</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="29.5" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1037,7 +1151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29.2" customHeight="1" thickBot="1">
+    <row r="5" spans="1:16" ht="29.25" customHeight="1" thickBot="1">
       <c r="A5" s="16" t="s">
         <v>15</v>
       </c>
@@ -1060,15 +1174,20 @@
       <c r="G5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="I5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="J5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="36" customHeight="1" thickBot="1">
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="36" customHeight="1" thickBot="1">
       <c r="A6" s="21" t="s">
         <v>31</v>
       </c>
@@ -1087,18 +1206,24 @@
       <c r="F6" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="30"/>
+      <c r="G6" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>51</v>
+      </c>
       <c r="I6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="J6" s="31">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="14.65" thickBot="1">
+        <v>10000</v>
+      </c>
+      <c r="P6" s="4">
+        <f>P5+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15" thickBot="1">
       <c r="A7" s="21" t="s">
         <v>32</v>
       </c>
@@ -1120,15 +1245,21 @@
       <c r="G7" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="32"/>
+      <c r="H7" s="32" t="s">
+        <v>51</v>
+      </c>
       <c r="I7" s="32" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="31">
         <v>600</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="28.9" thickBot="1">
+      <c r="P7" s="4">
+        <f t="shared" ref="P7:P25" si="1">P6+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="29.5" thickBot="1">
       <c r="A8" s="21" t="s">
         <v>33</v>
       </c>
@@ -1150,15 +1281,21 @@
       <c r="G8" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="32"/>
+      <c r="H8" s="32" t="s">
+        <v>51</v>
+      </c>
       <c r="I8" s="32" t="s">
         <v>30</v>
       </c>
       <c r="J8" s="31">
         <v>600</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="14.65" thickBot="1">
+      <c r="P8" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15" thickBot="1">
       <c r="A9" s="21">
         <v>9</v>
       </c>
@@ -1188,10 +1325,14 @@
         <v>10000</v>
       </c>
       <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" ht="14.65" thickBot="1">
+      <c r="P9" s="4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15" thickBot="1">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B10" s="33">
         <v>1</v>
@@ -1200,60 +1341,73 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="34"/>
+      <c r="H10" s="40">
+        <v>1</v>
+      </c>
       <c r="I10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="35">
         <v>10000</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="14.65" thickBot="1">
+      <c r="K10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15" thickBot="1">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="36">
         <v>0.35</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="34" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="40">
         <v>1</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J11" s="39">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="14.65" thickBot="1">
+        <v>500</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15" thickBot="1">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="10">
         <v>1</v>
@@ -1262,30 +1416,37 @@
         <v>0.35</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="38">
+        <v>500</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15" thickBot="1">
+      <c r="A13" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="38">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="14.65" thickBot="1">
-      <c r="A13" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="B13" s="10">
         <v>1</v>
@@ -1294,30 +1455,37 @@
         <v>0.35</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G13" s="34" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J13" s="38">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="14.65" thickBot="1">
+        <v>500</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" thickBot="1">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="10">
         <v>1</v>
@@ -1326,25 +1494,347 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="34" t="s">
-        <v>59</v>
-      </c>
       <c r="H14" s="40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J14" s="38">
         <v>600</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" thickBot="1">
+      <c r="A15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="38">
+        <v>10000</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" thickBot="1">
+      <c r="A16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="33">
+        <v>1</v>
+      </c>
+      <c r="C16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="35">
+        <v>10000</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1">
+      <c r="A17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="33">
+        <v>1</v>
+      </c>
+      <c r="C17" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="40">
+        <v>3</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="35">
+        <v>10000</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" thickBot="1">
+      <c r="A18" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="33">
+        <v>1</v>
+      </c>
+      <c r="C18" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="40">
+        <v>2</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="35">
+        <v>10000</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" thickBot="1">
+      <c r="A19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1</v>
+      </c>
+      <c r="C19" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="35">
+        <v>10000</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1">
+      <c r="A20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="33">
+        <v>1</v>
+      </c>
+      <c r="C20" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="35">
+        <v>10000</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1">
+      <c r="A21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="33">
+        <v>1</v>
+      </c>
+      <c r="C21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="35">
+        <v>10000</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="18.75" customHeight="1" thickBot="1">
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1</v>
+      </c>
+      <c r="C22" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="4">
+        <v>510</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="P23" s="4">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="P24" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="P25" s="4">
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>